<commit_message>
Remove warnings from tests
</commit_message>
<xml_diff>
--- a/output2.xlsx
+++ b/output2.xlsx
@@ -822,10 +822,10 @@
         <v>85</v>
       </c>
       <c r="AD2">
-        <v>7.536221909247484</v>
+        <v>7.41818178187627</v>
       </c>
       <c r="AE2">
-        <v>7.576915412343151</v>
+        <v>7.399928440167592</v>
       </c>
     </row>
     <row r="3" spans="1:31">
@@ -914,10 +914,10 @@
         <v>-835102.45</v>
       </c>
       <c r="AD3">
-        <v>-844232.6938739994</v>
+        <v>-204943.4633497131</v>
       </c>
       <c r="AE3">
-        <v>-847062.5919435836</v>
+        <v>-201603.4482634706</v>
       </c>
     </row>
     <row r="4" spans="1:31">

</xml_diff>

<commit_message>
WIP - National accounts - volume
</commit_message>
<xml_diff>
--- a/output2.xlsx
+++ b/output2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>Country Ameco</t>
   </si>
@@ -53,228 +53,6 @@
   </si>
   <si>
     <t>Millions</t>
-  </si>
-  <si>
-    <t>4220.391057</t>
-  </si>
-  <si>
-    <t>3698</t>
-  </si>
-  <si>
-    <t>5961.842162</t>
-  </si>
-  <si>
-    <t>4257.912398</t>
-  </si>
-  <si>
-    <t>3687</t>
-  </si>
-  <si>
-    <t>5936.923173</t>
-  </si>
-  <si>
-    <t>4337.1</t>
-  </si>
-  <si>
-    <t>3715</t>
-  </si>
-  <si>
-    <t>6132.523519</t>
-  </si>
-  <si>
-    <t>4340.4</t>
-  </si>
-  <si>
-    <t>3738.1</t>
-  </si>
-  <si>
-    <t>6047.833653</t>
-  </si>
-  <si>
-    <t>4356.5</t>
-  </si>
-  <si>
-    <t>3762.2</t>
-  </si>
-  <si>
-    <t>6139.778269</t>
-  </si>
-  <si>
-    <t>4435.4</t>
-  </si>
-  <si>
-    <t>3810.4</t>
-  </si>
-  <si>
-    <t>6291.210236</t>
-  </si>
-  <si>
-    <t>4457.4</t>
-  </si>
-  <si>
-    <t>4007</t>
-  </si>
-  <si>
-    <t>6373.9565</t>
-  </si>
-  <si>
-    <t>4474.4</t>
-  </si>
-  <si>
-    <t>4092.65</t>
-  </si>
-  <si>
-    <t>6553.0809</t>
-  </si>
-  <si>
-    <t>4516.5</t>
-  </si>
-  <si>
-    <t>4055.625</t>
-  </si>
-  <si>
-    <t>6615.8992</t>
-  </si>
-  <si>
-    <t>4554.7</t>
-  </si>
-  <si>
-    <t>4069.825</t>
-  </si>
-  <si>
-    <t>6579.8233</t>
-  </si>
-  <si>
-    <t>4585.6</t>
-  </si>
-  <si>
-    <t>4070.375</t>
-  </si>
-  <si>
-    <t>6553.9888</t>
-  </si>
-  <si>
-    <t>4645.4</t>
-  </si>
-  <si>
-    <t>4138.95</t>
-  </si>
-  <si>
-    <t>6598.1005</t>
-  </si>
-  <si>
-    <t>4718.7</t>
-  </si>
-  <si>
-    <t>4235.425</t>
-  </si>
-  <si>
-    <t>6661.2194</t>
-  </si>
-  <si>
-    <t>4761.3</t>
-  </si>
-  <si>
-    <t>4263.975</t>
-  </si>
-  <si>
-    <t>6765.2164</t>
-  </si>
-  <si>
-    <t>4804</t>
-  </si>
-  <si>
-    <t>4380.275</t>
-  </si>
-  <si>
-    <t>6896.1374</t>
-  </si>
-  <si>
-    <t>4863.9</t>
-  </si>
-  <si>
-    <t>4445.875</t>
-  </si>
-  <si>
-    <t>6990.9625</t>
-  </si>
-  <si>
-    <t>4903.6</t>
-  </si>
-  <si>
-    <t>4420.7</t>
-  </si>
-  <si>
-    <t>6882.1499</t>
-  </si>
-  <si>
-    <t>4959.1</t>
-  </si>
-  <si>
-    <t>4488.725</t>
-  </si>
-  <si>
-    <t>6916.1241</t>
-  </si>
-  <si>
-    <t>4961.3</t>
-  </si>
-  <si>
-    <t>4509.275</t>
-  </si>
-  <si>
-    <t>7073.3621</t>
-  </si>
-  <si>
-    <t>5003.6</t>
-  </si>
-  <si>
-    <t>4523.9</t>
-  </si>
-  <si>
-    <t>7105.3676</t>
-  </si>
-  <si>
-    <t>5035.9</t>
-  </si>
-  <si>
-    <t>4530.3</t>
-  </si>
-  <si>
-    <t>7073.5119</t>
-  </si>
-  <si>
-    <t>5060.9</t>
-  </si>
-  <si>
-    <t>4543.55</t>
-  </si>
-  <si>
-    <t>7091.5676</t>
-  </si>
-  <si>
-    <t>5099.7</t>
-  </si>
-  <si>
-    <t>4551.625</t>
-  </si>
-  <si>
-    <t>7105.8235</t>
-  </si>
-  <si>
-    <t>5125.4</t>
-  </si>
-  <si>
-    <t>4586.7</t>
-  </si>
-  <si>
-    <t>7200.5608</t>
-  </si>
-  <si>
-    <t>5154.7</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -746,87 +524,6 @@
       <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M2" t="s">
-        <v>37</v>
-      </c>
-      <c r="N2" t="s">
-        <v>40</v>
-      </c>
-      <c r="O2" t="s">
-        <v>43</v>
-      </c>
-      <c r="P2" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>49</v>
-      </c>
-      <c r="R2" t="s">
-        <v>52</v>
-      </c>
-      <c r="S2" t="s">
-        <v>55</v>
-      </c>
-      <c r="T2" t="s">
-        <v>58</v>
-      </c>
-      <c r="U2" t="s">
-        <v>61</v>
-      </c>
-      <c r="V2" t="s">
-        <v>64</v>
-      </c>
-      <c r="W2" t="s">
-        <v>67</v>
-      </c>
-      <c r="X2" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AD2">
-        <v>7.41818178187627</v>
-      </c>
-      <c r="AE2">
-        <v>7.399928440167592</v>
-      </c>
     </row>
     <row r="3" spans="1:31">
       <c r="A3" t="s">
@@ -933,81 +630,6 @@
       <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" t="s">
-        <v>32</v>
-      </c>
-      <c r="L4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M4" t="s">
-        <v>38</v>
-      </c>
-      <c r="N4" t="s">
-        <v>41</v>
-      </c>
-      <c r="O4" t="s">
-        <v>44</v>
-      </c>
-      <c r="P4" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>50</v>
-      </c>
-      <c r="R4" t="s">
-        <v>53</v>
-      </c>
-      <c r="S4" t="s">
-        <v>56</v>
-      </c>
-      <c r="T4" t="s">
-        <v>59</v>
-      </c>
-      <c r="U4" t="s">
-        <v>62</v>
-      </c>
-      <c r="V4" t="s">
-        <v>65</v>
-      </c>
-      <c r="W4" t="s">
-        <v>68</v>
-      </c>
-      <c r="X4" t="s">
-        <v>71</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>83</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>86</v>
-      </c>
     </row>
     <row r="5" spans="1:31">
       <c r="A5" t="s">
@@ -1021,81 +643,6 @@
       </c>
       <c r="D5" t="s">
         <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L5" t="s">
-        <v>36</v>
-      </c>
-      <c r="M5" t="s">
-        <v>39</v>
-      </c>
-      <c r="N5" t="s">
-        <v>42</v>
-      </c>
-      <c r="O5" t="s">
-        <v>45</v>
-      </c>
-      <c r="P5" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>51</v>
-      </c>
-      <c r="R5" t="s">
-        <v>54</v>
-      </c>
-      <c r="S5" t="s">
-        <v>57</v>
-      </c>
-      <c r="T5" t="s">
-        <v>60</v>
-      </c>
-      <c r="U5" t="s">
-        <v>63</v>
-      </c>
-      <c r="V5" t="s">
-        <v>66</v>
-      </c>
-      <c r="W5" t="s">
-        <v>69</v>
-      </c>
-      <c r="X5" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>81</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>84</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:31">

</xml_diff>

<commit_message>
WIP - National Accounts Volume
</commit_message>
<xml_diff>
--- a/output2.xlsx
+++ b/output2.xlsx
@@ -610,11 +610,14 @@
       <c r="AB3">
         <v>-835102.45</v>
       </c>
+      <c r="AC3">
+        <v>-819041.3058870928</v>
+      </c>
       <c r="AD3">
-        <v>-204943.4633497131</v>
+        <v>-805886.7339426123</v>
       </c>
       <c r="AE3">
-        <v>-201603.4482634706</v>
+        <v>-792931.6265268835</v>
       </c>
     </row>
     <row r="4" spans="1:31">

</xml_diff>